<commit_message>
fixes #27 Regenerated outputs for ES, SHS, PHR CIFMM-2399 - add must support flag to onset and note elements - Summary Statement of Allergy or Intolerance
</commit_message>
<xml_diff>
--- a/output/EventSummary/allergyintolerance-summary-1.xlsx
+++ b/output/EventSummary/allergyintolerance-summary-1.xlsx
@@ -3835,7 +3835,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" hidden="true">
+    <row r="25">
       <c r="A25" t="s" s="2">
         <v>216</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>50</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>42</v>
@@ -4369,7 +4369,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" hidden="true">
+    <row r="30">
       <c r="A30" t="s" s="2">
         <v>250</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>41</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>42</v>

</xml_diff>

<commit_message>
Regenerate ES IG outputs
</commit_message>
<xml_diff>
--- a/output/EventSummary/allergyintolerance-summary-1.xlsx
+++ b/output/EventSummary/allergyintolerance-summary-1.xlsx
@@ -341,7 +341,7 @@
 </t>
   </si>
   <si>
-    <t>Related person that recorded the sensitivity</t>
+    <t>Recorder as a related person</t>
   </si>
   <si>
     <t>Reference to related person that recorded the record and takes responsibility for its content.</t>
@@ -352,7 +352,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-ait-02:A related person shall conform to Base RelatedPerson {AllergyIntolerance.extension('http://hl7.org.au/fhir/StructureDefinition/recorder-related-person').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-dh-base-1')}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-ait-02:A related person shall conform to Base RelatedPerson {AllergyIntolerance.extension('http://hl7.org.au/fhir/StructureDefinition/recorder-related-person').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-dh-base-1')}</t>
   </si>
   <si>
     <t>AllergyIntolerance.modifierExtension</t>

</xml_diff>

<commit_message>
Regenerate SHS, ES, PHR and SML outputs after merge
</commit_message>
<xml_diff>
--- a/output/EventSummary/allergyintolerance-summary-1.xlsx
+++ b/output/EventSummary/allergyintolerance-summary-1.xlsx
@@ -175,7 +175,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">id {[]} {[]}
+    <t xml:space="preserve">id
 </t>
   </si>
   <si>
@@ -194,7 +194,7 @@
     <t>AllergyIntolerance.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">Meta {[]} {[]}
+    <t xml:space="preserve">Meta
 </t>
   </si>
   <si>
@@ -210,7 +210,7 @@
     <t>AllergyIntolerance.implicitRules</t>
   </si>
   <si>
-    <t xml:space="preserve">uri {[]} {[]}
+    <t xml:space="preserve">uri
 </t>
   </si>
   <si>
@@ -230,7 +230,7 @@
     <t>AllergyIntolerance.language</t>
   </si>
   <si>
-    <t xml:space="preserve">code {[]} {[]}
+    <t xml:space="preserve">code
 </t>
   </si>
   <si>
@@ -262,7 +262,7 @@
 htmlxhtmldisplay</t>
   </si>
   <si>
-    <t xml:space="preserve">Narrative {[]} {[]}
+    <t xml:space="preserve">Narrative
 </t>
   </si>
   <si>
@@ -292,7 +292,7 @@
 anonymous resourcescontained resources</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource {[]} {[]}
+    <t xml:space="preserve">Resource
 </t>
   </si>
   <si>
@@ -314,7 +314,7 @@
     <t>AllergyIntolerance.extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[]} {[]}
+    <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
@@ -337,11 +337,11 @@
     <t>recorderRelatedPerson</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://hl7.org.au/fhir/StructureDefinition/recorder-related-person]]} {[]}
+    <t xml:space="preserve">Extension {http://hl7.org.au/fhir/StructureDefinition/recorder-related-person}
 </t>
   </si>
   <si>
-    <t>Recorder as a related person</t>
+    <t>Related person that recorded the sensitivity</t>
   </si>
   <si>
     <t>Reference to related person that recorded the record and takes responsibility for its content.</t>
@@ -377,7 +377,7 @@
     <t>AllergyIntolerance.identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifier {[]} {[]}
+    <t xml:space="preserve">Identifier
 </t>
   </si>
   <si>
@@ -542,7 +542,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">CodeableConcept {[]} {[]}
+    <t xml:space="preserve">CodeableConcept
 </t>
   </si>
   <si>
@@ -590,7 +590,7 @@
     <t>AllergyIntolerance.code.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string {[]} {[]}
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
@@ -624,7 +624,7 @@
     <t>AllergyIntolerance.code.coding</t>
   </si>
   <si>
-    <t xml:space="preserve">Coding {[]} {[]}
+    <t xml:space="preserve">Coding
 </t>
   </si>
   <si>
@@ -693,7 +693,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1]]}
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1)
 </t>
   </si>
   <si>
@@ -715,8 +715,8 @@
     <t>AllergyIntolerance.onset[x]</t>
   </si>
   <si>
-    <t>dateTime {[]} {[]}
-Age {[]} {[]}Period {[]} {[]}Range {[]} {[]}string {[]} {[]}</t>
+    <t>dateTime
+AgePeriodRange</t>
   </si>
   <si>
     <t>When allergy or intolerance was identified</t>
@@ -734,7 +734,7 @@
     <t>AllergyIntolerance.assertedDate</t>
   </si>
   <si>
-    <t xml:space="preserve">dateTime {[]} {[]}
+    <t xml:space="preserve">dateTime
 </t>
   </si>
   <si>
@@ -760,7 +760,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-dh-base-1], CanonicalType[http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-dh-base-1]]}
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-dh-base-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-dh-base-1)
 </t>
   </si>
   <si>
@@ -783,7 +783,7 @@
 Informant</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Patient], CanonicalType[http://hl7.org/fhir/StructureDefinition/RelatedPerson], CanonicalType[http://hl7.org/fhir/StructureDefinition/Practitioner]]}
+    <t xml:space="preserve">Reference(Patient|RelatedPerson|Practitioner)
 </t>
   </si>
   <si>
@@ -823,7 +823,7 @@
     <t>AllergyIntolerance.note</t>
   </si>
   <si>
-    <t xml:space="preserve">Annotation {[]} {[]}
+    <t xml:space="preserve">Annotation
 </t>
   </si>
   <si>
@@ -842,7 +842,7 @@
     <t>AllergyIntolerance.reaction</t>
   </si>
   <si>
-    <t xml:space="preserve">BackboneElement {[]} {[]}
+    <t xml:space="preserve">BackboneElement
 </t>
   </si>
   <si>
@@ -1098,67 +1098,67 @@
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin"/>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin"/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin"/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
   </borders>
@@ -1194,7 +1194,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM51"/>
+  <dimension ref="A1:AL51"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>

</xml_diff>

<commit_message>
Build  Advance Care Records, Event SUmmary, Personal Health Records, Prescription and Dispense Lists, Shared Health Summary and Shared Medicines List.
</commit_message>
<xml_diff>
--- a/output/EventSummary/allergyintolerance-summary-1.xlsx
+++ b/output/EventSummary/allergyintolerance-summary-1.xlsx
@@ -334,14 +334,14 @@
     <t>DomainResource.extension</t>
   </si>
   <si>
-    <t>recorderRelatedPerson</t>
+    <t>authorRelatedPerson</t>
   </si>
   <si>
     <t xml:space="preserve">Extension {http://hl7.org.au/fhir/StructureDefinition/author-related-person}
 </t>
   </si>
   <si>
-    <t>Related person that recorded the sensitivity</t>
+    <t>Related person that authored the resource</t>
   </si>
   <si>
     <t>Reference to related person that authored the resource and takes responsibility for its content.</t>
@@ -1091,7 +1091,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="42.24609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.78125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="20.07421875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>

</xml_diff>